<commit_message>
Sort - add columns - add filters - improvement
</commit_message>
<xml_diff>
--- a/NewsWebsite/wwwroot/excel_templetes/amlak_info.xlsx
+++ b/NewsWebsite/wwwroot/excel_templetes/amlak_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\ASP\Erp_Project\NewsWebsite\wwwroot\excel_templetes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C10D53A-04B3-4A92-80A2-5E8F7FF0A185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{971380E9-4B5D-42AB-BDE1-0E4001165F5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7F283721-637C-4500-B8C0-83D034281840}"/>
   </bookViews>
@@ -49,9 +49,6 @@
     <t>اطلاعات تکیل شده؟</t>
   </si>
   <si>
-    <t>مساخت</t>
-  </si>
-  <si>
     <t>نوع</t>
   </si>
   <si>
@@ -64,19 +61,22 @@
     <t>ساختار</t>
   </si>
   <si>
-    <t>مالک</t>
-  </si>
-  <si>
-    <t>Latitude</t>
-  </si>
-  <si>
-    <t>Longitude</t>
-  </si>
-  <si>
     <t>کد کاربری</t>
   </si>
   <si>
     <t>نوع کاربری</t>
+  </si>
+  <si>
+    <t>متولی</t>
+  </si>
+  <si>
+    <t>مساحت</t>
+  </si>
+  <si>
+    <t>نوع مالکت</t>
+  </si>
+  <si>
+    <t>مختصات</t>
   </si>
 </sst>
 </file>
@@ -447,18 +447,18 @@
   <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.28515625" customWidth="1"/>
-    <col min="7" max="7" width="22.42578125" customWidth="1"/>
-    <col min="8" max="12" width="13.28515625" customWidth="1"/>
+    <col min="1" max="2" width="8.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.28515625" customWidth="1"/>
+    <col min="8" max="8" width="22.42578125" customWidth="1"/>
+    <col min="9" max="12" width="13.28515625" customWidth="1"/>
     <col min="13" max="13" width="14.7109375" customWidth="1"/>
     <col min="14" max="14" width="13.28515625" customWidth="1"/>
   </cols>
@@ -468,43 +468,43 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>